<commit_message>
Refined documentation and the coding comments
</commit_message>
<xml_diff>
--- a/documentations/1.2 Detailed Design.xlsx
+++ b/documentations/1.2 Detailed Design.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/Desktop/download/Massey/NZLife/CVs/cover letter/Westpac/assessment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/projects/SimpleWeatherInformationService/documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5AB00E-4E0D-504F-821D-4F566ABAF93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAE237D-CCFA-3D44-9142-630D6FAD6754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="27900" windowHeight="16460" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="27900" windowHeight="16460" activeTab="3" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pojo" sheetId="9" r:id="rId1"/>
+    <sheet name="Pojo &amp; Exception" sheetId="9" r:id="rId1"/>
     <sheet name="controller layer " sheetId="1" r:id="rId2"/>
     <sheet name="service layer" sheetId="3" r:id="rId3"/>
     <sheet name="Repositor_ DAO layer" sheetId="5" r:id="rId4"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="125">
   <si>
     <t>WeatherInformationController</t>
   </si>
@@ -98,11 +98,6 @@
   </si>
   <si>
     <t>availableService</t>
-  </si>
-  <si>
-    <t>1. Return all avaiable services to user
-2. Mapoed to the uri "/""
-3. jakarta.servlet.http.HttpServletResponse do not need iuput from client side, this is defualt input from Spring Framework</t>
   </si>
   <si>
     <t>co.nz.westpac.interview.simpleweatherinformationservice.service;</t>
@@ -406,58 +401,78 @@
     <t>method to be implemented in the implementation class fro get the available cities' name</t>
   </si>
   <si>
-    <t>1, Getting the request from service layer
+    <t>1. Mapoed to the uri "/queryweatherbycities"
+2. Accept the list of city as query request from clients 
+3. if the cities amount &gt;3, get  INPUT_EXCEED_MESSAGE from MessageUtil and return to the client
+4. If the cities amount = 0, get  NO_INPUT_CITY_MESSAGE from MessageUtil and return to client
+5. Otherwise, pass cities information to service layer, call WeatherInformationService's  queryWeatherByCities method to get value then return the result to the client
+6. If Service Exception  thrown from the service layer,
+get  SERVICE_EXCEPTION_MESSAGE from MessageUtil and return to client 
+7. If DataQueryException Exception is thrown from the service layer,
+get  DAO_EXCEPTION_MESSAGE from MessageUtil and return to the client 
+8. if other Exceptions thrown from the service layer,
+get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to the client 
+9. jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
+  </si>
+  <si>
+    <t>1. Mapoed to the uri "/availablecities"
+2. call WeatherInformationService's  queryWeatherByCities method to get  all available cities for weather information query, return to client-side
+3. if ServiceException is thrown from service layer,
+get  SERVICE_EXCEPTION_MESSAGE from MessageUtil and return to client 
+4. If DataQueryExceptionis thrown from the service layer,
+get  DAO_EXCEPTION_MESSAGE from MessageUtil and return to the client 
+5. if other Exceptions thrown from the service layer,
+get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to the client 
+6. jakarta.servlet.http.HttpServletResponse do not need input from the client side, this is the default input from Spring Framework</t>
+  </si>
+  <si>
+    <t>1. Mapoed to the uri "/""
+2. Return a simple manual to the client
+3. jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
+  </si>
+  <si>
+    <t>1. Accepting the list of cities as a query from the controller side
+2. Passing the cities information to WeatherRecordDao, call queryWeatherByCities method
+3. Getting the result  from WeatherRecordDao, Add the date information for each valid weather information 
+4.  Return the value to the controller layer
+5. if WeatherRecordDao return any exceptions, throw to the controller layer
+6. If ServiceException or any Exception occurred,  throw to the controller layer</t>
+  </si>
+  <si>
+    <t>1. Accepting the request from controller side
+2. Passing the cities information to WeatherRecordDao, call getAvailableCities method
+3.  Return the value to the controller layer
+4. if WeatherRecordDao return any exceptions, throw to the controller
+5. If ServiceException or any Exception occurred,  throw to the controller</t>
+  </si>
+  <si>
+    <t>1. Accepting the list of cities as a query request from the service layer
+2. Loop cities information, for each city get the city name, for each, call MockedDatabase's getWeatherByCity() method to get the query result 
+3. If the result is not null, put it into the return  list
+4. If the result is  null, call WeatherRecordUtil.createWeatherRecordForNotExistCity to get a weather in formation with the city not available tips
+5. Return the result list to the service Layer
+6. If DataQueryException or any Exception occurs,  throw it to the service layer</t>
+  </si>
+  <si>
+    <t>1, Getting the request from the service layer
 2. call MockedDatabase's getAvailableCities method to get available cities' data
-3. return data to service layer
-4. If DataQueryException or any Exception occurred,  throw to service layer</t>
-  </si>
-  <si>
-    <t>1. Accepting the list of city as  query from service layer
-2. Loop cities information, get city name, for each, call MockedDatabase's getWeatherByCity() method to get the query result 
-3. if result is not null, put it into return  list
-4.  if result is  null, call WeatherRecordUtil.createWeatherRecordForNotExistCity to get a weather in formation with city not avaibale tips
-5. Return result list to service Layer
-6. If DataQueryException or any Exception occurred,  throw to service layer</t>
-  </si>
-  <si>
-    <t>1. Accepting the list of city as  query from controller side
-2. Passing the cities information to WeatherRecordDao, call queryWeatherByCities method
-3. Getting the result  fron WeatherRecordDao, Add the date information for each vaild wearther information 
-4.  Return the value to controller layer
-5. if WeatherRecordDao return any excceptions, throw to controller
-6. If ServiceException or any Exception occurred,  throw to controller</t>
-  </si>
-  <si>
-    <t>1. Accepting the list of city as  query from controller side
-2. Passing the cities information to WeatherRecordDao, call getAvailableCities method
-3.  Return the value to controller layer
-4. if WeatherRecordDao return any excceptions, throw to controller
-5. If ServiceException or any Exception occurred,  throw to controller</t>
-  </si>
-  <si>
-    <t>1. Mapoed to the uri "/queryweatherbycities"
-2. Accept the list of city as  query from clients 
-3. if the cities amount &gt;3, get  INPUT_EXCEED_MESSAGE from MessageUtil and return to client
-4. If the cities amount = 0, get  NO_INPUT_CITY_MESSAGE from MessageUtil and return to client
-5. Other wise, pass cities inforation to service layer, call WeatherInformationService's  queryWeatherByCities method to get value then return the result to client
-6. if Service Exception  thrown from service layer,
-get  SERVICE_EXCEPTION_MESSAGE from MessageUtil and return to client 
-7. if Repository/DAO Exception  thrown from service layer,
-get  DAO_EXCEPTION_MESSAGE from MessageUtil and return to client 
-8. if other Exception  thrown from service layer,
-get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to client 
-9. jakarta.servlet.http.HttpServletResponse do not need iuput from client side, this is defualt input from Spring Framework</t>
-  </si>
-  <si>
-    <t>1. Mapoed to the uri "/availablecities"
-2. call WeatherInformationService's  queryWeatherByCities method get  all avaiable cities for weather information query, return to client side
-3. if Service Exception  thrown from service layer,
-get  SERVICE_EXCEPTION_MESSAGE from MessageUtil and return to client 
-4. if Repository/DAO Exception  thrown from service layer,
-get  DAO_EXCEPTION_MESSAGE from MessageUtil and return to client 
-5. if other Exception  thrown from service layer,
-get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to client 
-6. jakarta.servlet.http.HttpServletResponse do not need iuput from client side, this is defualt input from Spring Framework</t>
+3. return data to the service layer
+4. If DataQueryException or any Exception occurred,  throw to the service layer</t>
+  </si>
+  <si>
+    <t>co.nz.westpac.interview.simpleweatherinformationservice.Exceptions</t>
+  </si>
+  <si>
+    <t>DataQueryException</t>
+  </si>
+  <si>
+    <t>Customized Exception for exception occurred in dao layer</t>
+  </si>
+  <si>
+    <t>ServiceException</t>
+  </si>
+  <si>
+    <t>ustomized Exception for exception occurred in service layer</t>
   </si>
 </sst>
 </file>
@@ -557,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -565,9 +580,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -597,9 +609,22 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,321 +959,383 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115DC55E-9174-DF40-931C-7803CBFD96CD}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B50" sqref="B50"/>
+      <selection pane="topRight" activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="72.83203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="56.83203125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="26.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="72.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="56.83203125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="23" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="10"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="B32" s="23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="18" t="s">
+      <c r="B33" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C35" s="17" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="7" t="s">
+    <row r="36" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A36" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="B39" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="18" t="s">
+      <c r="C39" s="13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10" t="s">
+    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="51" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="C41" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="10"/>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="10"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="14" t="s">
+      <c r="B45" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="14" t="s">
+      <c r="B46" s="23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="102" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="14" t="s">
+      <c r="B47" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="14" t="s">
+      <c r="B51" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
+      <c r="B52" s="23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C39" s="14" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A41" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>103</v>
+      <c r="B53" s="6" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -1260,9 +1347,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CF29C3-6CCF-5E40-B7B3-48E005714D48}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G10" sqref="G10"/>
+      <selection pane="topRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1271,11 +1358,11 @@
     <col min="2" max="2" width="72" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="42.83203125" customWidth="1"/>
-    <col min="5" max="5" width="40" customWidth="1"/>
+    <col min="5" max="5" width="43.33203125" style="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1283,15 +1370,15 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1299,10 +1386,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1315,23 +1402,23 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="16" t="s">
+      <c r="C8" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1342,13 +1429,13 @@
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="323" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="293" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1359,10 +1446,10 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>119</v>
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
@@ -1376,10 +1463,10 @@
         <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1391,9 +1478,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530541A8-86E8-6440-91A5-C91B7ED15BC0}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C24" sqref="C24"/>
+      <selection pane="topRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1406,43 +1493,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="C5" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1454,13 +1541,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1469,51 +1556,51 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+      <c r="A11" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>35</v>
+      <c r="B12" s="12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1521,39 +1608,39 @@
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="C19" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="153" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="170" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1561,27 +1648,27 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="119" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="136" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>117</v>
       </c>
     </row>
@@ -1594,9 +1681,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B6D489-6F2E-434C-86EF-267FE6BF2BFB}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A21" sqref="A21"/>
+      <selection pane="topRight" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1609,43 +1696,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="C5" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1657,13 +1744,13 @@
         <v>14</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1672,51 +1759,51 @@
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
-        <v>104</v>
+      <c r="A13" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1724,39 +1811,39 @@
       <c r="B15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="C19" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="187" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="188" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>12</v>
       </c>
@@ -1764,13 +1851,13 @@
         <v>14</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>115</v>
+        <v>32</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="102" x14ac:dyDescent="0.2">
@@ -1780,10 +1867,10 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>114</v>
+        <v>32</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1797,7 +1884,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C10" sqref="C10"/>
+      <selection pane="topRight" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1810,324 +1897,324 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="16" t="s">
+      <c r="C9" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="5" t="s">
-        <v>49</v>
+      <c r="C11" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="13" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="16" t="s">
+      <c r="C19" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B25" s="13" t="s">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="16" t="s">
+      <c r="C28" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>110</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="16" t="s">
+      <c r="C35" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B41" s="13" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update readme and detailed design document
</commit_message>
<xml_diff>
--- a/documentations/1.2 Detailed Design.xlsx
+++ b/documentations/1.2 Detailed Design.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/projects/SimpleWeatherInformationService/documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAE237D-CCFA-3D44-9142-630D6FAD6754}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A2C540-A416-3C4C-9E8C-F9A10666D899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="27900" windowHeight="16460" activeTab="3" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="27900" windowHeight="16460" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
   </bookViews>
   <sheets>
-    <sheet name="Pojo &amp; Exception" sheetId="9" r:id="rId1"/>
-    <sheet name="controller layer " sheetId="1" r:id="rId2"/>
-    <sheet name="service layer" sheetId="3" r:id="rId3"/>
-    <sheet name="Repositor_ DAO layer" sheetId="5" r:id="rId4"/>
-    <sheet name="Utils &amp; Constants" sheetId="7" r:id="rId5"/>
+    <sheet name="Spring Framework" sheetId="11" r:id="rId1"/>
+    <sheet name="Pojo &amp; Exception" sheetId="9" r:id="rId2"/>
+    <sheet name="controller layer " sheetId="1" r:id="rId3"/>
+    <sheet name="service layer" sheetId="3" r:id="rId4"/>
+    <sheet name="Repositor_ DAO layer" sheetId="5" r:id="rId5"/>
+    <sheet name="Utils &amp; Constants" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="131">
   <si>
     <t>WeatherInformationController</t>
   </si>
@@ -473,6 +474,24 @@
   </si>
   <si>
     <t>ustomized Exception for exception occurred in service layer</t>
+  </si>
+  <si>
+    <t>SimpleWeatherInformationServiceApplication</t>
+  </si>
+  <si>
+    <t>co.nz.westpac.interview.simpleweatherinformationservice</t>
+  </si>
+  <si>
+    <t>City class used for start the application</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>String[]</t>
+  </si>
+  <si>
+    <t>Excute this for initial the in-memory database and start the application</t>
   </si>
 </sst>
 </file>
@@ -958,12 +977,82 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3DE262-5779-5D41-9E7A-F5AA61D5FC2A}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.5" style="7" customWidth="1"/>
+    <col min="3" max="3" width="72.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="56.83203125" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115DC55E-9174-DF40-931C-7803CBFD96CD}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B58" sqref="B58"/>
+      <selection pane="topRight" activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1343,13 +1432,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CF29C3-6CCF-5E40-B7B3-48E005714D48}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E18" sqref="E18"/>
+      <selection pane="topRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,7 +1563,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{530541A8-86E8-6440-91A5-C91B7ED15BC0}">
   <dimension ref="A1:E21"/>
   <sheetViews>
@@ -1677,11 +1766,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B6D489-6F2E-434C-86EF-267FE6BF2BFB}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="E24" sqref="E24"/>
     </sheetView>
@@ -1878,7 +1967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{733CCE45-27B2-E14A-A1F2-A31BA049C60F}">
   <dimension ref="A1:E42"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added input/output log supprt, the function assumed as side system was implemented already and do not need designed in this time Contoller and documents updated following this change
</commit_message>
<xml_diff>
--- a/documentations/1.2 Detailed Design.xlsx
+++ b/documentations/1.2 Detailed Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/projects/SimpleWeatherInformationService/documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04DA178-79A2-5B49-ADE9-8068F61976A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53DE04D-8AA5-6D4A-BB3F-8B5DE7753334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="500" windowWidth="27900" windowHeight="16460" activeTab="1" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
+    <workbookView xWindow="420" yWindow="500" windowWidth="27900" windowHeight="16420" activeTab="2" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Framework" sheetId="11" r:id="rId1"/>
@@ -82,17 +82,10 @@
     <t>queryWeatherByCities</t>
   </si>
   <si>
-    <t>jakarta.servlet.http.HttpServletResponse</t>
-  </si>
-  <si>
     <t xml:space="preserve">java.util.List&lt;co.nz.westpac.interview.simpleweatherinformationservice.pojo.City&gt; </t>
   </si>
   <si>
     <t>org.springframework.http.ResponseEntity&lt;Object&gt;</t>
-  </si>
-  <si>
-    <t>java.util.List&lt;co.nz.westpac.interview.simpleweatherinformationservice.pojo.City&gt; 
-jakarta.servlet.http.HttpServletResponse</t>
   </si>
   <si>
     <t>getAvailableCities</t>
@@ -400,6 +393,96 @@
   </si>
   <si>
     <t>method to be implemented in the implementation class fro get the available cities' name</t>
+  </si>
+  <si>
+    <t>1. Accepting the list of cities as a query from the controller side
+2. Passing the cities information to WeatherRecordDao, call queryWeatherByCities method
+3. Getting the result  from WeatherRecordDao, Add the date information for each valid weather information 
+4.  Return the value to the controller layer
+5. if WeatherRecordDao return any exceptions, throw to the controller layer
+6. If ServiceException or any Exception occurred,  throw to the controller layer</t>
+  </si>
+  <si>
+    <t>1. Accepting the request from controller side
+2. Passing the cities information to WeatherRecordDao, call getAvailableCities method
+3.  Return the value to the controller layer
+4. if WeatherRecordDao return any exceptions, throw to the controller
+5. If ServiceException or any Exception occurred,  throw to the controller</t>
+  </si>
+  <si>
+    <t>1. Accepting the list of cities as a query request from the service layer
+2. Loop cities information, for each city get the city name, for each, call MockedDatabase's getWeatherByCity() method to get the query result 
+3. If the result is not null, put it into the return  list
+4. If the result is  null, call WeatherRecordUtil.createWeatherRecordForNotExistCity to get a weather in formation with the city not available tips
+5. Return the result list to the service Layer
+6. If DataQueryException or any Exception occurs,  throw it to the service layer</t>
+  </si>
+  <si>
+    <t>co.nz.westpac.interview.simpleweatherinformationservice.Exceptions</t>
+  </si>
+  <si>
+    <t>DataQueryException</t>
+  </si>
+  <si>
+    <t>Customized Exception for exception occurred in dao layer</t>
+  </si>
+  <si>
+    <t>ServiceException</t>
+  </si>
+  <si>
+    <t>ustomized Exception for exception occurred in service layer</t>
+  </si>
+  <si>
+    <t>SimpleWeatherInformationServiceApplication</t>
+  </si>
+  <si>
+    <t>co.nz.westpac.interview.simpleweatherinformationservice</t>
+  </si>
+  <si>
+    <t>City class used for start the application</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>String[]</t>
+  </si>
+  <si>
+    <t>Excute this for initial the in-memory database and start the application</t>
+  </si>
+  <si>
+    <t>1, Getting the request from the service layer
+2. Call MockedDatabase's getAvailableCities method to get available cities' data
+3. Return data to the service layer
+4. If DataQueryException or any Exception occurred,  throw to the service layer</t>
+  </si>
+  <si>
+    <t>Logic/Comments</t>
+  </si>
+  <si>
+    <t>java.util.List&lt;co.nz.westpac.interview.simpleweatherinformationservice.pojo.City&gt; 
+jakarta.servlet.http.HttpServletRequest
+jakarta.servlet.http.HttpServletResponse</t>
+  </si>
+  <si>
+    <t>jakarta.servlet.http.HttpServletRequest
+jakarta.servlet.http.HttpServletResponse</t>
+  </si>
+  <si>
+    <t>1. Mapoed to the uri "/""
+2. Return a simple manual to the client
+3. jakarta.servlet.http.HttpServletRequest and jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
+  </si>
+  <si>
+    <t>1. Mapoed to the uri "/availablecities"
+2. call WeatherInformationService's  queryWeatherByCities method to get  all available cities for weather information query, return to client-side
+3. if ServiceException is thrown from service layer,
+get  SERVICE_EXCEPTION_MESSAGE from MessageUtil and return to client 
+4. If DataQueryExceptionis thrown from the service layer,
+get  DAO_EXCEPTION_MESSAGE from MessageUtil and return to the client 
+5. if other Exceptions thrown from the service layer,
+get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to the client 
+6. jakarta.servlet.http.HttpServletRequest and jakarta.servlet.http.HttpServletResponse do not need input from the client side, this is the default input from Spring Framework</t>
   </si>
   <si>
     <t>1. Mapoed to the uri "/queryweatherbycities"
@@ -413,88 +496,7 @@
 get  DAO_EXCEPTION_MESSAGE from MessageUtil and return to the client 
 8. if other Exceptions thrown from the service layer,
 get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to the client 
-9. jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
-  </si>
-  <si>
-    <t>1. Mapoed to the uri "/availablecities"
-2. call WeatherInformationService's  queryWeatherByCities method to get  all available cities for weather information query, return to client-side
-3. if ServiceException is thrown from service layer,
-get  SERVICE_EXCEPTION_MESSAGE from MessageUtil and return to client 
-4. If DataQueryExceptionis thrown from the service layer,
-get  DAO_EXCEPTION_MESSAGE from MessageUtil and return to the client 
-5. if other Exceptions thrown from the service layer,
-get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to the client 
-6. jakarta.servlet.http.HttpServletResponse do not need input from the client side, this is the default input from Spring Framework</t>
-  </si>
-  <si>
-    <t>1. Mapoed to the uri "/""
-2. Return a simple manual to the client
-3. jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
-  </si>
-  <si>
-    <t>1. Accepting the list of cities as a query from the controller side
-2. Passing the cities information to WeatherRecordDao, call queryWeatherByCities method
-3. Getting the result  from WeatherRecordDao, Add the date information for each valid weather information 
-4.  Return the value to the controller layer
-5. if WeatherRecordDao return any exceptions, throw to the controller layer
-6. If ServiceException or any Exception occurred,  throw to the controller layer</t>
-  </si>
-  <si>
-    <t>1. Accepting the request from controller side
-2. Passing the cities information to WeatherRecordDao, call getAvailableCities method
-3.  Return the value to the controller layer
-4. if WeatherRecordDao return any exceptions, throw to the controller
-5. If ServiceException or any Exception occurred,  throw to the controller</t>
-  </si>
-  <si>
-    <t>1. Accepting the list of cities as a query request from the service layer
-2. Loop cities information, for each city get the city name, for each, call MockedDatabase's getWeatherByCity() method to get the query result 
-3. If the result is not null, put it into the return  list
-4. If the result is  null, call WeatherRecordUtil.createWeatherRecordForNotExistCity to get a weather in formation with the city not available tips
-5. Return the result list to the service Layer
-6. If DataQueryException or any Exception occurs,  throw it to the service layer</t>
-  </si>
-  <si>
-    <t>co.nz.westpac.interview.simpleweatherinformationservice.Exceptions</t>
-  </si>
-  <si>
-    <t>DataQueryException</t>
-  </si>
-  <si>
-    <t>Customized Exception for exception occurred in dao layer</t>
-  </si>
-  <si>
-    <t>ServiceException</t>
-  </si>
-  <si>
-    <t>ustomized Exception for exception occurred in service layer</t>
-  </si>
-  <si>
-    <t>SimpleWeatherInformationServiceApplication</t>
-  </si>
-  <si>
-    <t>co.nz.westpac.interview.simpleweatherinformationservice</t>
-  </si>
-  <si>
-    <t>City class used for start the application</t>
-  </si>
-  <si>
-    <t>main</t>
-  </si>
-  <si>
-    <t>String[]</t>
-  </si>
-  <si>
-    <t>Excute this for initial the in-memory database and start the application</t>
-  </si>
-  <si>
-    <t>1, Getting the request from the service layer
-2. Call MockedDatabase's getAvailableCities method to get available cities' data
-3. Return data to the service layer
-4. If DataQueryException or any Exception occurred,  throw to the service layer</t>
-  </si>
-  <si>
-    <t>Logic/Comments</t>
+9. jakarta.servlet.http.HttpServletRequest and jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
   </si>
 </sst>
 </file>
@@ -986,7 +988,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -994,7 +996,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1002,7 +1004,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1010,7 +1012,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>6</v>
@@ -1018,13 +1020,13 @@
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1036,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115DC55E-9174-DF40-931C-7803CBFD96CD}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView topLeftCell="A41" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C39" sqref="C39"/>
     </sheetView>
@@ -1056,7 +1058,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1064,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1072,15 +1074,15 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>6</v>
@@ -1088,21 +1090,21 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>6</v>
@@ -1110,22 +1112,22 @@
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1140,7 +1142,7 @@
         <v>2</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1148,7 +1150,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1156,15 +1158,15 @@
         <v>7</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>6</v>
@@ -1172,65 +1174,65 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>6</v>
@@ -1238,22 +1240,22 @@
     </row>
     <row r="26" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1268,7 +1270,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1276,7 +1278,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
@@ -1284,15 +1286,15 @@
         <v>7</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>6</v>
@@ -1300,32 +1302,32 @@
     </row>
     <row r="36" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" s="9" t="s">
         <v>94</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>6</v>
@@ -1333,22 +1335,22 @@
     </row>
     <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1363,7 +1365,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1371,7 +1373,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1379,7 +1381,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1394,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1402,7 +1404,7 @@
         <v>1</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1410,7 +1412,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1422,9 +1424,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CF29C3-6CCF-5E40-B7B3-48E005714D48}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E8" sqref="E8"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1484,64 +1486,64 @@
         <v>11</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="323" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="293" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
+      <c r="B11" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1572,12 +1574,12 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>5</v>
@@ -1588,7 +1590,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1599,13 +1601,13 @@
         <v>11</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1613,31 +1615,31 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1651,7 +1653,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1659,15 +1661,15 @@
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1675,7 +1677,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1692,10 +1694,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1706,13 +1708,13 @@
         <v>11</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="170" x14ac:dyDescent="0.2">
@@ -1720,16 +1722,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E20" s="19" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="136" x14ac:dyDescent="0.2">
@@ -1738,13 +1740,13 @@
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E21" s="19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1775,15 +1777,15 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1791,7 +1793,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -1802,10 +1804,10 @@
         <v>11</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>6</v>
@@ -1816,31 +1818,31 @@
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1854,7 +1856,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1862,15 +1864,15 @@
         <v>1</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1878,7 +1880,7 @@
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1895,10 +1897,10 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1909,13 +1911,13 @@
         <v>11</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="188" customHeight="1" x14ac:dyDescent="0.2">
@@ -1923,29 +1925,29 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1976,7 +1978,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1984,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1992,15 +1994,15 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C5" s="16" t="s">
         <v>6</v>
@@ -2008,24 +2010,24 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -2036,37 +2038,37 @@
         <v>11</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -2081,7 +2083,7 @@
         <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -2089,7 +2091,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -2097,7 +2099,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -2108,28 +2110,28 @@
         <v>11</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -2144,7 +2146,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -2152,7 +2154,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -2160,15 +2162,15 @@
         <v>7</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>6</v>
@@ -2176,57 +2178,57 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -2237,28 +2239,28 @@
         <v>11</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -2273,7 +2275,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -2281,7 +2283,7 @@
         <v>1</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -2289,7 +2291,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added customized 400 and 404 exception handle, let return information more friendly when these expcetion occurred, modified assumptions and detailed design Adjust detailed design and comments for code in DAO of query data from mocked database
</commit_message>
<xml_diff>
--- a/documentations/1.2 Detailed Design.xlsx
+++ b/documentations/1.2 Detailed Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/projects/SimpleWeatherInformationService/documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53DE04D-8AA5-6D4A-BB3F-8B5DE7753334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9629DE68-D7C9-734D-BC07-985D6AC31DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="500" windowWidth="27900" windowHeight="16420" activeTab="2" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
+    <workbookView xWindow="420" yWindow="500" windowWidth="27900" windowHeight="16420" activeTab="4" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Framework" sheetId="11" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Repositor_ DAO layer" sheetId="5" r:id="rId5"/>
     <sheet name="Utils &amp; Constants" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="140">
   <si>
     <t>WeatherInformationController</t>
   </si>
@@ -408,14 +408,6 @@
 3.  Return the value to the controller layer
 4. if WeatherRecordDao return any exceptions, throw to the controller
 5. If ServiceException or any Exception occurred,  throw to the controller</t>
-  </si>
-  <si>
-    <t>1. Accepting the list of cities as a query request from the service layer
-2. Loop cities information, for each city get the city name, for each, call MockedDatabase's getWeatherByCity() method to get the query result 
-3. If the result is not null, put it into the return  list
-4. If the result is  null, call WeatherRecordUtil.createWeatherRecordForNotExistCity to get a weather in formation with the city not available tips
-5. Return the result list to the service Layer
-6. If DataQueryException or any Exception occurs,  throw it to the service layer</t>
   </si>
   <si>
     <t>co.nz.westpac.interview.simpleweatherinformationservice.Exceptions</t>
@@ -498,12 +490,64 @@
 get  UNKNOW_EXCEPTION_MESSAGE from MessageUtil and return to the client 
 9. jakarta.servlet.http.HttpServletRequest and jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
   </si>
+  <si>
+    <t>WeatherInformationExceptionHandelController</t>
+  </si>
+  <si>
+    <t>A controller advice class to provide customized system level exception handle and make return information more friendly</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>handelHttpMessageNotReadableException</t>
+  </si>
+  <si>
+    <t>handelNotFoundException</t>
+  </si>
+  <si>
+    <t>org.springframework.http.ResponseEntity</t>
+  </si>
+  <si>
+    <t>If 400 Bad Request exception occurred wirth HttpMessageNotReadableException, call MessageUtil.getExceptionUnreadableMessage() then return with  status HttpStatus.BAD_REQUEST in ResponseEntity.</t>
+  </si>
+  <si>
+    <t>If 404 not found  exception occurred wirth HttpMessageNotReadableException, call MessageUtil.getExceptionNotFoundMessage() then return with status HttpStatus.BAD_NOT_FOUND in ResponseEntity</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Accepting the list of cities as a query request from the service layer
+2. Loop cities information, for each city get the city name, for each, call MockedDatabase's getWeatherByCity() method to get the query result </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow (Body)"/>
+      </rPr>
+      <t xml:space="preserve">(Waring: call databse in each here becaue of use mocked in memory database, when use real RDS, need be optimised to access database only once) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. If the result is not null, put it into the return  list
+4. If the result is  null, call WeatherRecordUtil.createWeatherRecordForNotExistCity to get a weather in formation with the city not available tips
+5. Return the result list to the service Layer
+6. If DataQueryException or any Exception occurs,  throw it to the service layer</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -530,6 +574,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow (Body)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -585,7 +634,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -632,6 +681,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -988,7 +1040,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -996,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1004,7 +1056,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,13 +1072,13 @@
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>123</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -1038,9 +1090,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115DC55E-9174-DF40-931C-7803CBFD96CD}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
+    <sheetView topLeftCell="A39" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C39" sqref="C39"/>
+      <selection pane="topRight" activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1365,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1373,7 +1425,7 @@
         <v>1</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1381,7 +1433,7 @@
         <v>7</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1396,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1404,7 +1456,7 @@
         <v>1</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1412,7 +1464,7 @@
         <v>7</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1422,11 +1474,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CF29C3-6CCF-5E40-B7B3-48E005714D48}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A14" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A9" sqref="A9:XFD9"/>
+      <selection pane="topRight" activeCell="D38" sqref="C38:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1492,15 +1544,15 @@
         <v>20</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>14</v>
@@ -1509,7 +1561,7 @@
         <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="323" x14ac:dyDescent="0.2">
@@ -1517,7 +1569,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
@@ -1526,7 +1578,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="102" x14ac:dyDescent="0.2">
@@ -1534,7 +1586,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>14</v>
@@ -1543,7 +1595,105 @@
         <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1607,7 +1757,7 @@
         <v>20</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="51" x14ac:dyDescent="0.2">
@@ -1714,7 +1864,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="170" x14ac:dyDescent="0.2">
@@ -1758,9 +1908,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B6D489-6F2E-434C-86EF-267FE6BF2BFB}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1917,7 +2067,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="188" customHeight="1" x14ac:dyDescent="0.2">
@@ -1934,7 +2084,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>113</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="102" x14ac:dyDescent="0.2">
@@ -1947,7 +2097,7 @@
         <v>30</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2044,7 +2194,7 @@
         <v>20</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -2116,7 +2266,7 @@
         <v>20</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="68" x14ac:dyDescent="0.2">
@@ -2245,7 +2395,7 @@
         <v>20</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="68" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Changed the exception handle class and detailed design, followed the calling Method limitation, for path "/" keep all methods for easier success
</commit_message>
<xml_diff>
--- a/documentations/1.2 Detailed Design.xlsx
+++ b/documentations/1.2 Detailed Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewzhu/projects/SimpleWeatherInformationService/documentations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9629DE68-D7C9-734D-BC07-985D6AC31DF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D756CEFE-D038-5541-AEA8-ED3DD0FC8809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="500" windowWidth="27900" windowHeight="16420" activeTab="4" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
+    <workbookView xWindow="420" yWindow="500" windowWidth="27900" windowHeight="16420" xr2:uid="{C4F7C2B9-1629-B94C-A59B-FF182AF2B448}"/>
   </bookViews>
   <sheets>
     <sheet name="Spring Framework" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="144">
   <si>
     <t>WeatherInformationController</t>
   </si>
@@ -491,9 +491,6 @@
 9. jakarta.servlet.http.HttpServletRequest and jakarta.servlet.http.HttpServletResponse do not need input from client side, this is default input from Spring Framework</t>
   </si>
   <si>
-    <t>WeatherInformationExceptionHandelController</t>
-  </si>
-  <si>
     <t>A controller advice class to provide customized system level exception handle and make return information more friendly</t>
   </si>
   <si>
@@ -510,9 +507,6 @@
   </si>
   <si>
     <t>If 400 Bad Request exception occurred wirth HttpMessageNotReadableException, call MessageUtil.getExceptionUnreadableMessage() then return with  status HttpStatus.BAD_REQUEST in ResponseEntity.</t>
-  </si>
-  <si>
-    <t>If 404 not found  exception occurred wirth HttpMessageNotReadableException, call MessageUtil.getExceptionNotFoundMessage() then return with status HttpStatus.BAD_NOT_FOUND in ResponseEntity</t>
   </si>
   <si>
     <r>
@@ -541,6 +535,24 @@
 5. Return the result list to the service Layer
 6. If DataQueryException or any Exception occurs,  throw it to the service layer</t>
     </r>
+  </si>
+  <si>
+    <t>WeatherInformationExceptionHandleControllerAdvice</t>
+  </si>
+  <si>
+    <t>If 405 method not support  exception occurred wirth HttpMessageNotReadableException, call MessageUtil.handleHttpRequestMethodNotSupportedException() then return with status HttpStatus.METHOD_NOT_ALLOWED in ResponseEntity</t>
+  </si>
+  <si>
+    <t>handleHttpRequestMethodNotSupportedException</t>
+  </si>
+  <si>
+    <t>A controller advice class to provide customized controller level exception handle and make return information more  friendly</t>
+  </si>
+  <si>
+    <t>public class GlobalExceptionHandleControllerAdvice</t>
+  </si>
+  <si>
+    <t>If 404 not found  exception occurred wirth HttpMessageNotReadableException, call MessageUtil.getExceptionNotFoundMessage() then return with status HttpStatus.NOT_FOUND in ResponseEntity</t>
   </si>
 </sst>
 </file>
@@ -1020,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED3DE262-5779-5D41-9E7A-F5AA61D5FC2A}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
@@ -1090,9 +1102,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{115DC55E-9174-DF40-931C-7803CBFD96CD}">
   <dimension ref="A1:E53"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A49" sqref="A49:XFD49"/>
+      <selection pane="topRight" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,11 +1486,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CF29C3-6CCF-5E40-B7B3-48E005714D48}">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D38" sqref="C38:D38"/>
+      <selection pane="topRight" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1618,7 +1630,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -1626,7 +1638,7 @@
         <v>7</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1639,10 +1651,10 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1664,36 +1676,117 @@
     </row>
     <row r="23" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="10"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="E35" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="102" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>138</v>
+      <c r="C36" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1908,7 +2001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B6D489-6F2E-434C-86EF-267FE6BF2BFB}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G20" sqref="G20"/>
     </sheetView>
@@ -2084,7 +2177,7 @@
         <v>30</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="102" x14ac:dyDescent="0.2">

</xml_diff>